<commit_message>
Actualización de Burndown Chart - Sprint 2
</commit_message>
<xml_diff>
--- a/Desarrollo/Edutec/Gestión/Sprint 2/Sprint Backlog - S2.xlsx
+++ b/Desarrollo/Edutec/Gestión/Sprint 2/Sprint Backlog - S2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Universidad\Edutec\Desarrollo\Edutec\Gestión\Sprint 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E01B5DB-2E0C-4332-9E9B-6EC532C4322D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7432C11B-D879-46BA-A368-919B95CC3C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint Backlog 2" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="122">
   <si>
     <t>Universidad Nacional Mayor de San Marcos</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>Tarea 1 (T01-T1)</t>
-  </si>
-  <si>
-    <t>Manuel Fajardo / Leyla Campos</t>
   </si>
   <si>
     <t>Tarea 3 (T01-T3)</t>
@@ -398,6 +395,15 @@
   <si>
     <t>Perfil de usuario</t>
   </si>
+  <si>
+    <t>C05</t>
+  </si>
+  <si>
+    <t>Angel Romaní  / Leyla Campos</t>
+  </si>
+  <si>
+    <t>Favoritos</t>
+  </si>
 </sst>
 </file>
 
@@ -466,7 +472,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -513,6 +519,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-4.9989318521683403E-2"/>
+        <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
   </fills>
@@ -788,7 +800,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -977,37 +989,6 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1042,6 +1023,52 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1259,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -1595,17 +1622,17 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A11" s="68" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="70"/>
+      <c r="A11" s="88" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="89"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="89"/>
+      <c r="H11" s="89"/>
+      <c r="I11" s="90"/>
       <c r="J11" s="3"/>
       <c r="K11" s="12"/>
       <c r="L11" s="3"/>
@@ -1626,19 +1653,19 @@
     </row>
     <row r="12" spans="1:26" ht="17.25" customHeight="1" thickBot="1">
       <c r="A12" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="26" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" s="25">
         <v>44537</v>
@@ -1650,7 +1677,7 @@
         <v>4</v>
       </c>
       <c r="I12" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1672,19 +1699,19 @@
     </row>
     <row r="13" spans="1:26" ht="17.25" customHeight="1" thickBot="1">
       <c r="A13" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>24</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="25">
         <v>44538</v>
@@ -1696,7 +1723,7 @@
         <v>4</v>
       </c>
       <c r="I13" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1718,19 +1745,19 @@
     </row>
     <row r="14" spans="1:26" ht="17.25" customHeight="1">
       <c r="A14" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>25</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" s="25">
         <v>44539</v>
@@ -1742,7 +1769,7 @@
         <v>8</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1764,19 +1791,19 @@
     </row>
     <row r="15" spans="1:26" ht="17.25" customHeight="1" thickBot="1">
       <c r="A15" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D15" s="24" t="s">
         <v>26</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" s="25">
         <v>44543</v>
@@ -1788,7 +1815,7 @@
         <v>4</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="14"/>
@@ -1810,19 +1837,19 @@
     </row>
     <row r="16" spans="1:26" ht="17.25" customHeight="1" thickBot="1">
       <c r="A16" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="37" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>25</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F16" s="33">
         <v>44544</v>
@@ -1834,7 +1861,7 @@
         <v>4</v>
       </c>
       <c r="I16" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
@@ -1856,19 +1883,19 @@
     </row>
     <row r="17" spans="1:26" ht="17.25" customHeight="1" thickBot="1">
       <c r="A17" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="37" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D17" s="32" t="s">
         <v>26</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F17" s="33">
         <v>44545</v>
@@ -1880,7 +1907,7 @@
         <v>4</v>
       </c>
       <c r="I17" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="14"/>
@@ -1900,33 +1927,33 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A18" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="B18" s="16" t="s">
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A18" s="69" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="D18" s="18" t="s">
+      <c r="C18" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="17">
+      <c r="E18" s="73" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="74">
         <v>44546</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="74">
         <v>44547</v>
       </c>
-      <c r="H18" s="16">
-        <v>2</v>
-      </c>
-      <c r="I18" s="18" t="s">
-        <v>101</v>
+      <c r="H18" s="70">
+        <v>4</v>
+      </c>
+      <c r="I18" s="72" t="s">
+        <v>100</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -1947,32 +1974,32 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A19" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="B19" s="16" t="s">
+      <c r="A19" s="69" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="D19" s="18" t="s">
+      <c r="C19" s="75" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="17">
+      <c r="E19" s="73" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="74">
         <v>44547</v>
       </c>
-      <c r="G19" s="17">
+      <c r="G19" s="74">
         <v>44551</v>
       </c>
-      <c r="H19" s="16">
+      <c r="H19" s="71">
         <v>4</v>
       </c>
-      <c r="I19" s="18" t="s">
-        <v>101</v>
+      <c r="I19" s="72" t="s">
+        <v>100</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1993,31 +2020,31 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A20" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="B20" s="16" t="s">
+      <c r="A20" s="69" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="D20" s="18" t="s">
+      <c r="C20" s="77" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" s="17">
+      <c r="E20" s="78" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="79">
         <v>44551</v>
       </c>
-      <c r="G20" s="17">
+      <c r="G20" s="79">
         <v>44552</v>
       </c>
-      <c r="H20" s="16">
-        <v>2</v>
-      </c>
-      <c r="I20" s="18" t="s">
+      <c r="H20" s="76">
+        <v>4</v>
+      </c>
+      <c r="I20" s="78" t="s">
         <v>21</v>
       </c>
       <c r="J20" s="3"/>
@@ -2039,31 +2066,31 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A21" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="B21" s="16" t="s">
+      <c r="A21" s="69" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="D21" s="18" t="s">
+      <c r="C21" s="75" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" s="17">
-        <v>44551</v>
-      </c>
-      <c r="G21" s="17">
+      <c r="E21" s="73" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" s="74">
         <v>44552</v>
       </c>
-      <c r="H21" s="16">
-        <v>2</v>
-      </c>
-      <c r="I21" s="18" t="s">
+      <c r="G21" s="74">
+        <v>44553</v>
+      </c>
+      <c r="H21" s="71">
+        <v>4</v>
+      </c>
+      <c r="I21" s="72" t="s">
         <v>21</v>
       </c>
       <c r="J21" s="3"/>
@@ -2085,31 +2112,31 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A22" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="B22" s="19" t="s">
+      <c r="A22" s="69" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="D22" s="18" t="s">
+      <c r="C22" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="17">
-        <v>44552</v>
-      </c>
-      <c r="G22" s="17">
+      <c r="E22" s="73" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="74">
         <v>44553</v>
       </c>
-      <c r="H22" s="19">
+      <c r="G22" s="74">
+        <v>44554</v>
+      </c>
+      <c r="H22" s="70">
         <v>4</v>
       </c>
-      <c r="I22" s="18" t="s">
+      <c r="I22" s="72" t="s">
         <v>21</v>
       </c>
       <c r="J22" s="3"/>
@@ -2130,33 +2157,33 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A23" s="86" t="s">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A23" s="97" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23" s="98" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="98" t="s">
         <v>107</v>
       </c>
-      <c r="B23" s="87" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="88" t="s">
-        <v>113</v>
-      </c>
-      <c r="D23" s="89" t="s">
+      <c r="D23" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="90" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23" s="91">
+      <c r="E23" s="99" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="100">
         <v>44546</v>
       </c>
-      <c r="G23" s="91">
+      <c r="G23" s="100">
         <v>44547</v>
       </c>
-      <c r="H23" s="87">
-        <v>4</v>
-      </c>
-      <c r="I23" s="89" t="s">
-        <v>101</v>
+      <c r="H23" s="98">
+        <v>2</v>
+      </c>
+      <c r="I23" s="99" t="s">
+        <v>100</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -2177,32 +2204,32 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A24" s="86" t="s">
-        <v>107</v>
-      </c>
-      <c r="B24" s="92" t="s">
+      <c r="A24" s="97" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="92" t="s">
-        <v>114</v>
-      </c>
-      <c r="D24" s="89" t="s">
+      <c r="C24" s="98" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="90" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" s="91">
+      <c r="E24" s="99" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="100">
         <v>44547</v>
       </c>
-      <c r="G24" s="91">
+      <c r="G24" s="100">
         <v>44551</v>
       </c>
-      <c r="H24" s="88">
+      <c r="H24" s="98">
         <v>4</v>
       </c>
-      <c r="I24" s="89" t="s">
-        <v>101</v>
+      <c r="I24" s="99" t="s">
+        <v>100</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -2223,31 +2250,31 @@
       <c r="Z24" s="3"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A25" s="86" t="s">
-        <v>107</v>
-      </c>
-      <c r="B25" s="93" t="s">
+      <c r="A25" s="97" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="94" t="s">
-        <v>115</v>
-      </c>
-      <c r="D25" s="95" t="s">
+      <c r="C25" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="95" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25" s="96">
+      <c r="E25" s="99" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="100">
         <v>44551</v>
       </c>
-      <c r="G25" s="96">
+      <c r="G25" s="100">
         <v>44552</v>
       </c>
-      <c r="H25" s="93">
-        <v>4</v>
-      </c>
-      <c r="I25" s="95" t="s">
+      <c r="H25" s="98">
+        <v>2</v>
+      </c>
+      <c r="I25" s="99" t="s">
         <v>21</v>
       </c>
       <c r="J25" s="3"/>
@@ -2269,31 +2296,31 @@
       <c r="Z25" s="3"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A26" s="86" t="s">
-        <v>107</v>
-      </c>
-      <c r="B26" s="92" t="s">
+      <c r="A26" s="97" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="92" t="s">
-        <v>116</v>
-      </c>
-      <c r="D26" s="89" t="s">
+      <c r="C26" s="98" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="90" t="s">
-        <v>36</v>
-      </c>
-      <c r="F26" s="91">
+      <c r="E26" s="99" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="100">
+        <v>44551</v>
+      </c>
+      <c r="G26" s="100">
         <v>44552</v>
       </c>
-      <c r="G26" s="91">
-        <v>44553</v>
-      </c>
-      <c r="H26" s="88">
-        <v>4</v>
-      </c>
-      <c r="I26" s="89" t="s">
+      <c r="H26" s="98">
+        <v>2</v>
+      </c>
+      <c r="I26" s="99" t="s">
         <v>21</v>
       </c>
       <c r="J26" s="3"/>
@@ -2315,31 +2342,31 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A27" s="86" t="s">
-        <v>107</v>
-      </c>
-      <c r="B27" s="92" t="s">
+      <c r="A27" s="97" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="92" t="s">
-        <v>117</v>
-      </c>
-      <c r="D27" s="90" t="s">
+      <c r="C27" s="98" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="90" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" s="91">
+      <c r="E27" s="99" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="100">
+        <v>44552</v>
+      </c>
+      <c r="G27" s="100">
         <v>44553</v>
       </c>
-      <c r="G27" s="91">
-        <v>44554</v>
-      </c>
-      <c r="H27" s="87">
+      <c r="H27" s="101">
         <v>4</v>
       </c>
-      <c r="I27" s="89" t="s">
+      <c r="I27" s="99" t="s">
         <v>21</v>
       </c>
       <c r="J27" s="3"/>
@@ -2361,17 +2388,33 @@
       <c r="Z27" s="3"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
+      <c r="A28" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F28" s="17">
+        <v>44546</v>
+      </c>
+      <c r="G28" s="17">
+        <v>44547</v>
+      </c>
+      <c r="H28" s="16">
+        <v>2</v>
+      </c>
+      <c r="I28" s="18" t="s">
+        <v>100</v>
+      </c>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
@@ -2390,16 +2433,34 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
     </row>
-    <row r="29" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
+    <row r="29" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A29" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F29" s="17">
+        <v>44547</v>
+      </c>
+      <c r="G29" s="17">
+        <v>44551</v>
+      </c>
+      <c r="H29" s="16">
+        <v>2</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>100</v>
+      </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
@@ -2418,16 +2479,34 @@
       <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
     </row>
-    <row r="30" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
+    <row r="30" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A30" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F30" s="17">
+        <v>44551</v>
+      </c>
+      <c r="G30" s="17">
+        <v>44552</v>
+      </c>
+      <c r="H30" s="16">
+        <v>2</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>21</v>
+      </c>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
@@ -2446,16 +2525,34 @@
       <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
     </row>
-    <row r="31" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
+    <row r="31" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A31" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F31" s="17">
+        <v>44551</v>
+      </c>
+      <c r="G31" s="17">
+        <v>44552</v>
+      </c>
+      <c r="H31" s="16">
+        <v>2</v>
+      </c>
+      <c r="I31" s="18" t="s">
+        <v>21</v>
+      </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
@@ -2474,18 +2571,34 @@
       <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
     </row>
-    <row r="32" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A32" s="75" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="76"/>
-      <c r="C32" s="76"/>
-      <c r="D32" s="72"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
+    <row r="32" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A32" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" s="17">
+        <v>44552</v>
+      </c>
+      <c r="G32" s="17">
+        <v>44553</v>
+      </c>
+      <c r="H32" s="19">
+        <v>2</v>
+      </c>
+      <c r="I32" s="18" t="s">
+        <v>21</v>
+      </c>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
@@ -2504,22 +2617,18 @@
       <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
     </row>
-    <row r="33" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A33" s="71" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" s="72"/>
-      <c r="C33" s="64" t="s">
-        <v>97</v>
-      </c>
-      <c r="D33" s="64" t="s">
-        <v>42</v>
-      </c>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
+    <row r="33" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
@@ -2539,16 +2648,10 @@
       <c r="Z33" s="3"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A34" s="73" t="s">
-        <v>118</v>
-      </c>
-      <c r="B34" s="74"/>
-      <c r="C34" s="85" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="40">
-        <v>20</v>
-      </c>
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
@@ -2573,16 +2676,10 @@
       <c r="Z34" s="3"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A35" s="73" t="s">
-        <v>44</v>
-      </c>
-      <c r="B35" s="74"/>
-      <c r="C35" s="85" t="s">
-        <v>35</v>
-      </c>
-      <c r="D35" s="40">
-        <v>8</v>
-      </c>
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
@@ -2607,16 +2704,10 @@
       <c r="Z35" s="3"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A36" s="73" t="s">
-        <v>106</v>
-      </c>
-      <c r="B36" s="74"/>
-      <c r="C36" s="85" t="s">
-        <v>105</v>
-      </c>
-      <c r="D36" s="40">
-        <v>14</v>
-      </c>
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
@@ -2641,16 +2732,12 @@
       <c r="Z36" s="3"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A37" s="73" t="s">
-        <v>119</v>
-      </c>
-      <c r="B37" s="74"/>
-      <c r="C37" s="85" t="s">
-        <v>107</v>
-      </c>
-      <c r="D37" s="40">
-        <v>20</v>
-      </c>
+      <c r="A37" s="80" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="81"/>
+      <c r="C37" s="81"/>
+      <c r="D37" s="82"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
@@ -2675,10 +2762,16 @@
       <c r="Z37" s="3"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
+      <c r="A38" s="91" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="82"/>
+      <c r="C38" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="64" t="s">
+        <v>41</v>
+      </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -2703,10 +2796,16 @@
       <c r="Z38" s="3"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
+      <c r="A39" s="86" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" s="87"/>
+      <c r="C39" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="40">
+        <v>20</v>
+      </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
@@ -2731,16 +2830,16 @@
       <c r="Z39" s="3"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A40" s="65" t="s">
-        <v>94</v>
-      </c>
-      <c r="B40" s="65" t="s">
-        <v>95</v>
-      </c>
-      <c r="C40" s="77" t="s">
-        <v>96</v>
-      </c>
-      <c r="D40" s="77"/>
+      <c r="A40" s="86" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="87"/>
+      <c r="C40" s="68" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="40">
+        <v>8</v>
+      </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
@@ -2765,16 +2864,16 @@
       <c r="Z40" s="3"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A41" s="66">
-        <v>44536</v>
-      </c>
-      <c r="B41" s="67">
-        <v>1</v>
-      </c>
-      <c r="C41" s="78" t="s">
-        <v>98</v>
-      </c>
-      <c r="D41" s="79"/>
+      <c r="A41" s="86" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="87"/>
+      <c r="C41" s="68" t="s">
+        <v>106</v>
+      </c>
+      <c r="D41" s="40">
+        <v>20</v>
+      </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
@@ -2799,10 +2898,16 @@
       <c r="Z41" s="3"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+      <c r="A42" s="86" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42" s="87"/>
+      <c r="C42" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="D42" s="40">
+        <v>14</v>
+      </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
@@ -2827,10 +2932,16 @@
       <c r="Z42" s="3"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+      <c r="A43" s="86" t="s">
+        <v>105</v>
+      </c>
+      <c r="B43" s="87"/>
+      <c r="C43" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="40">
+        <v>14</v>
+      </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
@@ -2911,10 +3022,16 @@
       <c r="Z45" s="3"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
+      <c r="A46" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" s="65" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="83" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46" s="83"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
@@ -2939,10 +3056,16 @@
       <c r="Z46" s="3"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
+      <c r="A47" s="66">
+        <v>44536</v>
+      </c>
+      <c r="B47" s="67">
+        <v>1</v>
+      </c>
+      <c r="C47" s="84" t="s">
+        <v>97</v>
+      </c>
+      <c r="D47" s="85"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -29286,7 +29409,7 @@
       <c r="Y987" s="3"/>
       <c r="Z987" s="3"/>
     </row>
-    <row r="988" spans="1:26" ht="15" customHeight="1">
+    <row r="988" spans="1:26" ht="15.75" customHeight="1">
       <c r="A988" s="3"/>
       <c r="B988" s="3"/>
       <c r="C988" s="3"/>
@@ -29296,8 +29419,25 @@
       <c r="G988" s="3"/>
       <c r="H988" s="3"/>
       <c r="I988" s="3"/>
-    </row>
-    <row r="989" spans="1:26" ht="15" customHeight="1">
+      <c r="J988" s="3"/>
+      <c r="K988" s="3"/>
+      <c r="L988" s="3"/>
+      <c r="M988" s="3"/>
+      <c r="N988" s="3"/>
+      <c r="O988" s="3"/>
+      <c r="P988" s="3"/>
+      <c r="Q988" s="3"/>
+      <c r="R988" s="3"/>
+      <c r="S988" s="3"/>
+      <c r="T988" s="3"/>
+      <c r="U988" s="3"/>
+      <c r="V988" s="3"/>
+      <c r="W988" s="3"/>
+      <c r="X988" s="3"/>
+      <c r="Y988" s="3"/>
+      <c r="Z988" s="3"/>
+    </row>
+    <row r="989" spans="1:26" ht="15.75" customHeight="1">
       <c r="A989" s="3"/>
       <c r="B989" s="3"/>
       <c r="C989" s="3"/>
@@ -29307,8 +29447,25 @@
       <c r="G989" s="3"/>
       <c r="H989" s="3"/>
       <c r="I989" s="3"/>
-    </row>
-    <row r="990" spans="1:26" ht="15" customHeight="1">
+      <c r="J989" s="3"/>
+      <c r="K989" s="3"/>
+      <c r="L989" s="3"/>
+      <c r="M989" s="3"/>
+      <c r="N989" s="3"/>
+      <c r="O989" s="3"/>
+      <c r="P989" s="3"/>
+      <c r="Q989" s="3"/>
+      <c r="R989" s="3"/>
+      <c r="S989" s="3"/>
+      <c r="T989" s="3"/>
+      <c r="U989" s="3"/>
+      <c r="V989" s="3"/>
+      <c r="W989" s="3"/>
+      <c r="X989" s="3"/>
+      <c r="Y989" s="3"/>
+      <c r="Z989" s="3"/>
+    </row>
+    <row r="990" spans="1:26" ht="15.75" customHeight="1">
       <c r="A990" s="3"/>
       <c r="B990" s="3"/>
       <c r="C990" s="3"/>
@@ -29318,8 +29475,25 @@
       <c r="G990" s="3"/>
       <c r="H990" s="3"/>
       <c r="I990" s="3"/>
-    </row>
-    <row r="991" spans="1:26" ht="15" customHeight="1">
+      <c r="J990" s="3"/>
+      <c r="K990" s="3"/>
+      <c r="L990" s="3"/>
+      <c r="M990" s="3"/>
+      <c r="N990" s="3"/>
+      <c r="O990" s="3"/>
+      <c r="P990" s="3"/>
+      <c r="Q990" s="3"/>
+      <c r="R990" s="3"/>
+      <c r="S990" s="3"/>
+      <c r="T990" s="3"/>
+      <c r="U990" s="3"/>
+      <c r="V990" s="3"/>
+      <c r="W990" s="3"/>
+      <c r="X990" s="3"/>
+      <c r="Y990" s="3"/>
+      <c r="Z990" s="3"/>
+    </row>
+    <row r="991" spans="1:26" ht="15.75" customHeight="1">
       <c r="A991" s="3"/>
       <c r="B991" s="3"/>
       <c r="C991" s="3"/>
@@ -29329,8 +29503,25 @@
       <c r="G991" s="3"/>
       <c r="H991" s="3"/>
       <c r="I991" s="3"/>
-    </row>
-    <row r="992" spans="1:26" ht="15" customHeight="1">
+      <c r="J991" s="3"/>
+      <c r="K991" s="3"/>
+      <c r="L991" s="3"/>
+      <c r="M991" s="3"/>
+      <c r="N991" s="3"/>
+      <c r="O991" s="3"/>
+      <c r="P991" s="3"/>
+      <c r="Q991" s="3"/>
+      <c r="R991" s="3"/>
+      <c r="S991" s="3"/>
+      <c r="T991" s="3"/>
+      <c r="U991" s="3"/>
+      <c r="V991" s="3"/>
+      <c r="W991" s="3"/>
+      <c r="X991" s="3"/>
+      <c r="Y991" s="3"/>
+      <c r="Z991" s="3"/>
+    </row>
+    <row r="992" spans="1:26" ht="15.75" customHeight="1">
       <c r="A992" s="3"/>
       <c r="B992" s="3"/>
       <c r="C992" s="3"/>
@@ -29340,8 +29531,25 @@
       <c r="G992" s="3"/>
       <c r="H992" s="3"/>
       <c r="I992" s="3"/>
-    </row>
-    <row r="993" spans="1:9" ht="15" customHeight="1">
+      <c r="J992" s="3"/>
+      <c r="K992" s="3"/>
+      <c r="L992" s="3"/>
+      <c r="M992" s="3"/>
+      <c r="N992" s="3"/>
+      <c r="O992" s="3"/>
+      <c r="P992" s="3"/>
+      <c r="Q992" s="3"/>
+      <c r="R992" s="3"/>
+      <c r="S992" s="3"/>
+      <c r="T992" s="3"/>
+      <c r="U992" s="3"/>
+      <c r="V992" s="3"/>
+      <c r="W992" s="3"/>
+      <c r="X992" s="3"/>
+      <c r="Y992" s="3"/>
+      <c r="Z992" s="3"/>
+    </row>
+    <row r="993" spans="1:26" ht="15.75" customHeight="1">
       <c r="A993" s="3"/>
       <c r="B993" s="3"/>
       <c r="C993" s="3"/>
@@ -29351,8 +29559,25 @@
       <c r="G993" s="3"/>
       <c r="H993" s="3"/>
       <c r="I993" s="3"/>
-    </row>
-    <row r="994" spans="1:9" ht="15" customHeight="1">
+      <c r="J993" s="3"/>
+      <c r="K993" s="3"/>
+      <c r="L993" s="3"/>
+      <c r="M993" s="3"/>
+      <c r="N993" s="3"/>
+      <c r="O993" s="3"/>
+      <c r="P993" s="3"/>
+      <c r="Q993" s="3"/>
+      <c r="R993" s="3"/>
+      <c r="S993" s="3"/>
+      <c r="T993" s="3"/>
+      <c r="U993" s="3"/>
+      <c r="V993" s="3"/>
+      <c r="W993" s="3"/>
+      <c r="X993" s="3"/>
+      <c r="Y993" s="3"/>
+      <c r="Z993" s="3"/>
+    </row>
+    <row r="994" spans="1:26" ht="15" customHeight="1">
       <c r="A994" s="3"/>
       <c r="B994" s="3"/>
       <c r="C994" s="3"/>
@@ -29363,7 +29588,7 @@
       <c r="H994" s="3"/>
       <c r="I994" s="3"/>
     </row>
-    <row r="995" spans="1:9" ht="15" customHeight="1">
+    <row r="995" spans="1:26" ht="15" customHeight="1">
       <c r="A995" s="3"/>
       <c r="B995" s="3"/>
       <c r="C995" s="3"/>
@@ -29374,7 +29599,7 @@
       <c r="H995" s="3"/>
       <c r="I995" s="3"/>
     </row>
-    <row r="996" spans="1:9" ht="15" customHeight="1">
+    <row r="996" spans="1:26" ht="15" customHeight="1">
       <c r="A996" s="3"/>
       <c r="B996" s="3"/>
       <c r="C996" s="3"/>
@@ -29385,7 +29610,7 @@
       <c r="H996" s="3"/>
       <c r="I996" s="3"/>
     </row>
-    <row r="997" spans="1:9" ht="15" customHeight="1">
+    <row r="997" spans="1:26" ht="15" customHeight="1">
       <c r="A997" s="3"/>
       <c r="B997" s="3"/>
       <c r="C997" s="3"/>
@@ -29396,17 +29621,84 @@
       <c r="H997" s="3"/>
       <c r="I997" s="3"/>
     </row>
+    <row r="998" spans="1:26" ht="15" customHeight="1">
+      <c r="A998" s="3"/>
+      <c r="B998" s="3"/>
+      <c r="C998" s="3"/>
+      <c r="D998" s="3"/>
+      <c r="E998" s="3"/>
+      <c r="F998" s="3"/>
+      <c r="G998" s="3"/>
+      <c r="H998" s="3"/>
+      <c r="I998" s="3"/>
+    </row>
+    <row r="999" spans="1:26" ht="15" customHeight="1">
+      <c r="A999" s="3"/>
+      <c r="B999" s="3"/>
+      <c r="C999" s="3"/>
+      <c r="D999" s="3"/>
+      <c r="E999" s="3"/>
+      <c r="F999" s="3"/>
+      <c r="G999" s="3"/>
+      <c r="H999" s="3"/>
+      <c r="I999" s="3"/>
+    </row>
+    <row r="1000" spans="1:26" ht="15" customHeight="1">
+      <c r="A1000" s="3"/>
+      <c r="B1000" s="3"/>
+      <c r="C1000" s="3"/>
+      <c r="D1000" s="3"/>
+      <c r="E1000" s="3"/>
+      <c r="F1000" s="3"/>
+      <c r="G1000" s="3"/>
+      <c r="H1000" s="3"/>
+      <c r="I1000" s="3"/>
+    </row>
+    <row r="1001" spans="1:26" ht="15" customHeight="1">
+      <c r="A1001" s="3"/>
+      <c r="B1001" s="3"/>
+      <c r="C1001" s="3"/>
+      <c r="D1001" s="3"/>
+      <c r="E1001" s="3"/>
+      <c r="F1001" s="3"/>
+      <c r="G1001" s="3"/>
+      <c r="H1001" s="3"/>
+      <c r="I1001" s="3"/>
+    </row>
+    <row r="1002" spans="1:26" ht="15" customHeight="1">
+      <c r="A1002" s="3"/>
+      <c r="B1002" s="3"/>
+      <c r="C1002" s="3"/>
+      <c r="D1002" s="3"/>
+      <c r="E1002" s="3"/>
+      <c r="F1002" s="3"/>
+      <c r="G1002" s="3"/>
+      <c r="H1002" s="3"/>
+      <c r="I1002" s="3"/>
+    </row>
+    <row r="1003" spans="1:26" ht="15" customHeight="1">
+      <c r="A1003" s="3"/>
+      <c r="B1003" s="3"/>
+      <c r="C1003" s="3"/>
+      <c r="D1003" s="3"/>
+      <c r="E1003" s="3"/>
+      <c r="F1003" s="3"/>
+      <c r="G1003" s="3"/>
+      <c r="H1003" s="3"/>
+      <c r="I1003" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="A35:B35"/>
+  <mergeCells count="10">
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A40:B40"/>
     <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A42:B42"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -29428,25 +29720,25 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>40</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="41" t="s">
         <v>45</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>46</v>
       </c>
       <c r="C2" s="41"/>
       <c r="D2" s="41"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="41" t="s">
         <v>27</v>
@@ -29456,15 +29748,15 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="41" t="s">
         <v>48</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="41" t="s">
         <v>19</v>
@@ -29472,26 +29764,26 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="41" t="s">
         <v>51</v>
-      </c>
-      <c r="B6" s="41" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="41" t="s">
         <v>53</v>
-      </c>
-      <c r="B7" s="41" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="41" t="s">
         <v>55</v>
-      </c>
-      <c r="B8" s="41" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1"/>
@@ -30530,7 +30822,7 @@
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -30543,14 +30835,14 @@
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -30573,7 +30865,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -30599,11 +30891,11 @@
     </row>
     <row r="8" spans="1:26">
       <c r="A8" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -30653,17 +30945,17 @@
       </c>
     </row>
     <row r="11" spans="1:26">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="70"/>
+      <c r="B11" s="89"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="89"/>
+      <c r="H11" s="89"/>
+      <c r="I11" s="90"/>
       <c r="K11" s="12"/>
     </row>
     <row r="12" spans="1:26" ht="17.25" customHeight="1">
@@ -30677,10 +30969,10 @@
         <v>28</v>
       </c>
       <c r="D12" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="48" t="s">
         <v>63</v>
-      </c>
-      <c r="E12" s="48" t="s">
-        <v>64</v>
       </c>
       <c r="F12" s="49">
         <v>44368</v>
@@ -30692,7 +30984,7 @@
         <v>6</v>
       </c>
       <c r="I12" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="17.25" customHeight="1">
@@ -30703,13 +30995,13 @@
         <v>20</v>
       </c>
       <c r="C13" s="53" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="54" t="s">
         <v>66</v>
-      </c>
-      <c r="E13" s="54" t="s">
-        <v>67</v>
       </c>
       <c r="F13" s="55">
         <v>44375</v>
@@ -30721,7 +31013,7 @@
         <v>4</v>
       </c>
       <c r="I13" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
@@ -30749,13 +31041,13 @@
         <v>20</v>
       </c>
       <c r="C14" s="47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" s="48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E14" s="48" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F14" s="49">
         <v>44377</v>
@@ -30767,24 +31059,24 @@
         <v>10</v>
       </c>
       <c r="I14" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="17.25" customHeight="1">
       <c r="A15" s="45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="47" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="51" t="s">
         <v>69</v>
-      </c>
-      <c r="D15" s="51" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="51" t="s">
-        <v>70</v>
       </c>
       <c r="F15" s="57">
         <v>44370</v>
@@ -30796,24 +31088,24 @@
         <v>9</v>
       </c>
       <c r="I15" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="17.25" customHeight="1">
       <c r="A16" s="56" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="46" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="48" t="s">
-        <v>72</v>
-      </c>
       <c r="E16" s="48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F16" s="49">
         <v>44372</v>
@@ -30825,24 +31117,24 @@
         <v>10</v>
       </c>
       <c r="I16" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="17.25" customHeight="1">
       <c r="A17" s="58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="50" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="59" t="s">
         <v>73</v>
-      </c>
-      <c r="D17" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="59" t="s">
-        <v>74</v>
       </c>
       <c r="F17" s="49">
         <v>44383</v>
@@ -30854,37 +31146,37 @@
         <v>6</v>
       </c>
       <c r="I17" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="17.25" customHeight="1">
-      <c r="A18" s="81" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="69"/>
-      <c r="C18" s="69"/>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="69"/>
-      <c r="H18" s="69"/>
-      <c r="I18" s="70"/>
+      <c r="A18" s="93" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="89"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="89"/>
+      <c r="F18" s="89"/>
+      <c r="G18" s="89"/>
+      <c r="H18" s="89"/>
+      <c r="I18" s="90"/>
     </row>
     <row r="19" spans="1:9" ht="17.25" customHeight="1">
       <c r="A19" s="58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="50" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D19" s="48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E19" s="59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F19" s="60">
         <v>44397</v>
@@ -30896,24 +31188,24 @@
         <v>10</v>
       </c>
       <c r="I19" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="17.25" customHeight="1">
       <c r="A20" s="56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="46" t="s">
+      <c r="D20" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="61" t="s">
         <v>78</v>
-      </c>
-      <c r="D20" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="61" t="s">
-        <v>79</v>
       </c>
       <c r="F20" s="57">
         <v>44407</v>
@@ -30925,24 +31217,24 @@
         <v>6</v>
       </c>
       <c r="I20" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="17.25" customHeight="1">
       <c r="A21" s="56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E21" s="61" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F21" s="57">
         <v>44410</v>
@@ -30954,24 +31246,24 @@
         <v>10</v>
       </c>
       <c r="I21" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="17.25" customHeight="1">
       <c r="A22" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="48" t="s">
         <v>81</v>
-      </c>
-      <c r="D22" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="48" t="s">
-        <v>82</v>
       </c>
       <c r="F22" s="57">
         <v>44415</v>
@@ -30983,24 +31275,24 @@
         <v>6</v>
       </c>
       <c r="I22" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="17.25" customHeight="1">
       <c r="A23" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" s="46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D23" s="48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E23" s="48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F23" s="57">
         <v>44418</v>
@@ -31012,24 +31304,24 @@
         <v>10</v>
       </c>
       <c r="I23" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="17.25" customHeight="1">
       <c r="A24" s="56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="46" t="s">
+      <c r="D24" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="48" t="s">
         <v>85</v>
-      </c>
-      <c r="D24" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="48" t="s">
-        <v>86</v>
       </c>
       <c r="F24" s="57">
         <v>44424</v>
@@ -31041,24 +31333,24 @@
         <v>6</v>
       </c>
       <c r="I24" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="17.25" customHeight="1">
       <c r="A25" s="56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C25" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="48" t="s">
         <v>87</v>
-      </c>
-      <c r="D25" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25" s="48" t="s">
-        <v>88</v>
       </c>
       <c r="F25" s="57">
         <v>44427</v>
@@ -31070,12 +31362,12 @@
         <v>10</v>
       </c>
       <c r="I25" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="17.25" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -31088,29 +31380,29 @@
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1"/>
     <row r="28" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A28" s="82" t="s">
+      <c r="A28" s="94" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="95"/>
+      <c r="C28" s="87"/>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A29" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="83"/>
-      <c r="C28" s="74"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A29" s="84" t="s">
+      <c r="B29" s="87"/>
+      <c r="C29" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="74"/>
-      <c r="C29" s="38" t="s">
+      <c r="D29" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="39" t="s">
+    </row>
+    <row r="30" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A30" s="92" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A30" s="80" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="74"/>
+      <c r="B30" s="87"/>
       <c r="C30" s="62" t="s">
         <v>27</v>
       </c>
@@ -31119,60 +31411,60 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A31" s="80" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31" s="74"/>
+      <c r="A31" s="92" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="87"/>
       <c r="C31" s="62" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D31" s="39">
         <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A32" s="80" t="s">
-        <v>90</v>
-      </c>
-      <c r="B32" s="74"/>
+      <c r="A32" s="92" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="87"/>
       <c r="C32" s="62" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D32" s="39">
         <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A33" s="80" t="s">
-        <v>91</v>
-      </c>
-      <c r="B33" s="74"/>
+      <c r="A33" s="92" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="87"/>
       <c r="C33" s="62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D33" s="63">
         <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A34" s="80" t="s">
-        <v>92</v>
-      </c>
-      <c r="B34" s="74"/>
+      <c r="A34" s="92" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="87"/>
       <c r="C34" s="62" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D34" s="63">
         <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A35" s="80" t="s">
-        <v>93</v>
-      </c>
-      <c r="B35" s="74"/>
+      <c r="A35" s="92" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="87"/>
       <c r="C35" s="62" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D35" s="63">
         <v>20</v>

</xml_diff>